<commit_message>
annadido calculo de proveedores
</commit_message>
<xml_diff>
--- a/src/informesGenerados/ResumenCDNT.xlsx
+++ b/src/informesGenerados/ResumenCDNT.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t>Mes</t>
   </si>
@@ -113,24 +113,24 @@
     <t>DTCM</t>
   </si>
   <si>
+    <t>DTHO</t>
+  </si>
+  <si>
+    <t>DTAR</t>
+  </si>
+  <si>
+    <t>DTVC</t>
+  </si>
+  <si>
+    <t>DTCF</t>
+  </si>
+  <si>
+    <t>DTMY</t>
+  </si>
+  <si>
     <t>DTMZ</t>
   </si>
   <si>
-    <t>DTAR</t>
-  </si>
-  <si>
-    <t>DTVC</t>
-  </si>
-  <si>
-    <t>DTHO</t>
-  </si>
-  <si>
-    <t>DTMY</t>
-  </si>
-  <si>
-    <t>DTCF</t>
-  </si>
-  <si>
     <t>DVLH</t>
   </si>
   <si>
@@ -239,6 +239,9 @@
     <t>Alambre de coser</t>
   </si>
   <si>
+    <t>Crucetas</t>
+  </si>
+  <si>
     <t>Postes</t>
   </si>
   <si>
@@ -263,10 +266,10 @@
     <t>11 Municipios</t>
   </si>
   <si>
+    <t>% Servicios Afectados</t>
+  </si>
+  <si>
     <t>Cant-Hechos</t>
-  </si>
-  <si>
-    <t>% Servicios Afectados</t>
   </si>
   <si>
     <t>Venezuela</t>
@@ -1091,7 +1094,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>2020: 61 hechos</c:v>
+            <c:v>2020: 64 hechos</c:v>
           </c:tx>
           <c:dLbls>
             <c:spPr>
@@ -1237,7 +1240,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
@@ -1249,13 +1252,13 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -1534,7 +1537,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>2020: 37 hechos</c:v>
+            <c:v>2020: 41 hechos</c:v>
           </c:tx>
           <c:dLbls>
             <c:spPr>
@@ -1665,19 +1668,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>3</c:v>
@@ -1977,7 +1980,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos para graficos'!$B$44</c:f>
+              <c:f>'Datos para graficos'!$B$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2046,7 +2049,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Datos para graficos'!$A$45:$A$52</c:f>
+              <c:f>'Datos para graficos'!$A$46:$A$53</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -2078,7 +2081,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos para graficos'!$B$45:$B$52</c:f>
+              <c:f>'Datos para graficos'!$B$46:$B$53</c:f>
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -2370,7 +2373,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos para graficos'!$B$15</c:f>
+              <c:f>'Datos para graficos'!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2424,7 +2427,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Datos para graficos'!$A$16:$A$24</c:f>
+              <c:f>'Datos para graficos'!$A$17:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -2459,7 +2462,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos para graficos'!$B$16:$B$24</c:f>
+              <c:f>'Datos para graficos'!$B$17:$B$25</c:f>
               <c:numCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -2540,7 +2543,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos para graficos'!$B$61</c:f>
+              <c:f>'Datos para graficos'!$B$62</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2594,7 +2597,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Datos para graficos'!$A$62:$A$67</c:f>
+              <c:f>'Datos para graficos'!$A$63:$A$68</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2620,7 +2623,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos para graficos'!$B$62:$B$67</c:f>
+              <c:f>'Datos para graficos'!$B$63:$B$68</c:f>
               <c:numCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2844,7 +2847,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos para graficos'!$A$24:$A$44</c:f>
+              <c:f>'Datos para graficos'!$A$25:$A$45</c:f>
               <c:numCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -3144,7 +3147,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos para graficos'!$A$67:$A$87</c:f>
+              <c:f>'Datos para graficos'!$A$68:$A$88</c:f>
               <c:numCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -4653,14 +4656,14 @@
         <v>2020</v>
       </c>
       <c r="B2" s="15">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C2" s="15">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D2" s="16">
         <f ca="1">B2+C2</f>
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" ht="26.25" customHeight="true">
@@ -4684,15 +4687,15 @@
       </c>
       <c r="B4" s="14" t="str">
         <f ca="1">IF(B3&gt;B2,(B3-B2)&amp;" más",IF(B2&gt;B3,(B2-B3)&amp;" menos","Igual"))</f>
-        <v>14 más</v>
+        <v>11 más</v>
       </c>
       <c r="C4" s="14" t="str">
         <f ca="1">IF(C3&gt;C2,(C3-C2)&amp;" más",IF(C2&gt;C3,(C2-C3)&amp;" menos","Igual"))</f>
-        <v>16 menos</v>
+        <v>20 menos</v>
       </c>
       <c r="D4" s="16" t="str">
         <f ca="1">IF(D3&gt;D2,(D3-D2)&amp;" más",IF(D2&gt;D3,(D2-D3)&amp;" menos","Igual"))</f>
-        <v>2 menos</v>
+        <v>9 menos</v>
       </c>
     </row>
     <row r="5" ht="26.25" customHeight="true">
@@ -4701,15 +4704,15 @@
       </c>
       <c r="B5" s="17" t="str">
         <f ca="1">IF(B3&lt;B2,ROUND(100*(B2-B3)/B2,0)  &amp;  "% Red",IF(B3=B2,0%,ROUND(100*(B3-B2)/B2,0) &amp; "% Inc"))</f>
-        <v>23% Inc</v>
+        <v>17% Inc</v>
       </c>
       <c r="C5" s="17" t="str">
         <f ca="1">IF(C3&lt;C2,ROUND(100*(C2-C3)/C2,0) &amp; "% Red",IF(C3=C2,0%,ROUND(100*(C3-C2)/C2,0) &amp; "% Inc"))</f>
-        <v>43% Red</v>
+        <v>49% Red</v>
       </c>
       <c r="D5" s="18" t="str">
         <f ca="1">IF(D3&lt;D2,ROUND(100*(D2-D3)/D2,0) &amp; "% Red",IF(D3=D2,0%,ROUND(100*(D3-D2)/D2,0) &amp; "% Inc"))</f>
-        <v>2% Red</v>
+        <v>9% Red</v>
       </c>
     </row>
     <row r="8">
@@ -4805,8 +4808,8 @@
       <c r="L10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="22">
-        <v>1</v>
+      <c r="M10" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -4898,23 +4901,23 @@
         <v>-11</v>
       </c>
       <c r="E13" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F13" s="7">
         <v>5</v>
       </c>
       <c r="G13" s="24">
         <f ca="1">F13-E13</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J13" s="22">
         <v>3</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="M13" s="24">
         <v>0</v>
@@ -4935,31 +4938,31 @@
         <v>3</v>
       </c>
       <c r="E14" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="7">
         <v>0</v>
       </c>
       <c r="G14" s="24">
         <f ca="1">F14-E14</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J14" s="22">
         <v>3</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="M14" s="24">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B15" s="7">
         <v>6</v>
@@ -4972,14 +4975,14 @@
         <v>3</v>
       </c>
       <c r="E15" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F15" s="7">
         <v>4</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="24">
         <f ca="1">F15-E15</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>38</v>
@@ -4988,7 +4991,7 @@
         <v>3</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="M15" s="24">
         <v>-1</v>
@@ -4996,7 +4999,7 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="7">
         <v>1</v>
@@ -5019,13 +5022,13 @@
         <v>0</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="J16" s="22">
         <v>2</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="M16" s="24">
         <v>-1</v>
@@ -5046,23 +5049,23 @@
         <v>4</v>
       </c>
       <c r="E17" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F17" s="7">
         <v>1</v>
       </c>
       <c r="G17" s="24">
         <f ca="1">F17-E17</f>
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="J17" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M17" s="24">
         <v>-1</v>
@@ -5073,14 +5076,14 @@
         <v>41</v>
       </c>
       <c r="B18" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" s="7">
         <v>2</v>
       </c>
       <c r="D18" s="25">
         <f ca="1">C18-B18</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E18" s="7">
         <v>3</v>
@@ -5099,10 +5102,10 @@
         <v>0</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="M18" s="24">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="19">
@@ -5130,13 +5133,13 @@
         <v>1</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J19" s="24">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="M19" s="24">
         <v>-2</v>
@@ -5167,13 +5170,13 @@
         <v>-2</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="J20" s="24">
         <v>-1</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="M20" s="24">
         <v>-2</v>
@@ -5204,13 +5207,13 @@
         <v>-1</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="J21" s="24">
         <v>-1</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="M21" s="24">
         <v>-2</v>
@@ -5218,17 +5221,17 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B22" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C22" s="7">
         <v>4</v>
       </c>
       <c r="D22" s="25">
         <f ca="1">C22-B22</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="E22" s="7">
         <v>1</v>
@@ -5241,10 +5244,10 @@
         <v>0</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J22" s="24">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="L22" s="7" t="s">
         <v>32</v>
@@ -5295,14 +5298,14 @@
         <v>40</v>
       </c>
       <c r="B24" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24" s="7">
         <v>12</v>
       </c>
       <c r="D24" s="23">
         <f ca="1">C24-B24</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" s="7">
         <v>2</v>
@@ -5324,7 +5327,7 @@
         <v>33</v>
       </c>
       <c r="M24" s="27">
-        <v>-4</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="25">
@@ -5383,9 +5386,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B8:D8"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" scale="100" paperSize="9" fitToWidth="1" fitToHeight="0" horizontalDpi="0" verticalDpi="0" copies="1"/>
@@ -5977,7 +5980,7 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B9" s="2">
         <f ca="1">SUM(C9:N9)</f>
@@ -6062,7 +6065,7 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2">
         <f ca="1">SUM(C10:N10)</f>
@@ -6572,7 +6575,7 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2">
         <f ca="1">SUM(C16:N16)</f>
@@ -7477,7 +7480,7 @@
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B27" s="2">
         <f ca="1">SUM(C27:N27)</f>
@@ -7562,7 +7565,7 @@
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28" s="2">
         <f ca="1">SUM(C28:N28)</f>
@@ -8072,7 +8075,7 @@
     </row>
     <row r="34">
       <c r="A34" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B34" s="2">
         <f ca="1">SUM(C34:N34)</f>
@@ -8827,12 +8830,12 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B1:N1"/>
+    <mergeCell ref="A3:AA3"/>
     <mergeCell ref="O1:AA1"/>
+    <mergeCell ref="B42:B53"/>
     <mergeCell ref="B54:B65"/>
-    <mergeCell ref="A3:AA3"/>
     <mergeCell ref="A21:AA21"/>
-    <mergeCell ref="B42:B53"/>
-    <mergeCell ref="B1:N1"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8843,7 +8846,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
   <sheetPr/>
-  <dimension ref="A1:A86"/>
+  <dimension ref="A1:A87"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScale="100" view="normal"/>
   </sheetViews>
@@ -8887,13 +8890,13 @@
         <v>64</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>794</v>
+        <v>854</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F4">
         <v>0.16</v>
@@ -8910,7 +8913,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F5">
         <v>0.08</v>
@@ -9012,7 +9015,7 @@
         <v>1070</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F11">
         <v>0.03</v>
@@ -9040,10 +9043,10 @@
         <v>73</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
         <v>30</v>
@@ -9057,10 +9060,10 @@
         <v>74</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
         <v>42</v>
@@ -9071,13 +9074,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>467</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
         <v>41</v>
@@ -9088,13 +9091,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C16">
-        <v>1122</v>
+        <v>467</v>
       </c>
       <c r="E16" t="s">
         <v>39</v>
@@ -9105,13 +9108,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>1122</v>
       </c>
       <c r="E17" t="s">
         <v>35</v>
@@ -9122,13 +9125,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>3460</v>
+        <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>40</v>
@@ -9139,33 +9142,33 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>3460</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F20">
         <v>6</v>
@@ -9173,16 +9176,16 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
         <v>2</v>
       </c>
-      <c r="C21">
-        <v>580</v>
-      </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F21">
         <v>3</v>
@@ -9190,16 +9193,16 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>7702</v>
+        <v>580</v>
       </c>
       <c r="E22" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F22">
         <v>2</v>
@@ -9207,16 +9210,16 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C23">
-        <v>3300</v>
+        <v>7702</v>
       </c>
       <c r="E23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -9224,21 +9227,27 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>72</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>3300</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F24" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
-        <v>6</v>
+      <c r="A25" t="s">
+        <v>83</v>
       </c>
       <c r="E25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F25">
         <v>1.69</v>
@@ -9246,10 +9255,10 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F26">
         <v>1.5</v>
@@ -9257,10 +9266,10 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -9268,10 +9277,10 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F28">
         <v>0.5</v>
@@ -9279,12 +9288,12 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
@@ -9294,47 +9303,47 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41">
@@ -9344,28 +9353,25 @@
     </row>
     <row r="42">
       <c r="A42">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
         <v>6</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
-        <v>75</v>
-      </c>
-      <c r="B44" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" t="s">
         <v>88</v>
-      </c>
-      <c r="B45">
-        <v>9</v>
       </c>
     </row>
     <row r="46">
@@ -9373,7 +9379,7 @@
         <v>89</v>
       </c>
       <c r="B46">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47">
@@ -9381,7 +9387,7 @@
         <v>90</v>
       </c>
       <c r="B47">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48">
@@ -9389,7 +9395,7 @@
         <v>91</v>
       </c>
       <c r="B48">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49">
@@ -9397,7 +9403,7 @@
         <v>92</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
@@ -9413,7 +9419,7 @@
         <v>94</v>
       </c>
       <c r="B51">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52">
@@ -9421,7 +9427,7 @@
         <v>95</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -9429,7 +9435,7 @@
         <v>96</v>
       </c>
       <c r="B53">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -9437,7 +9443,7 @@
         <v>97</v>
       </c>
       <c r="B54">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55">
@@ -9445,7 +9451,7 @@
         <v>98</v>
       </c>
       <c r="B55">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
@@ -9453,7 +9459,7 @@
         <v>99</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57">
@@ -9469,7 +9475,7 @@
         <v>101</v>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -9477,7 +9483,7 @@
         <v>102</v>
       </c>
       <c r="B59">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60">
@@ -9485,15 +9491,15 @@
         <v>103</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
@@ -9506,26 +9512,26 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B63">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B64">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66">
@@ -9533,17 +9539,20 @@
         <v>104</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
         <v>105</v>
       </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
     </row>
     <row r="68">
-      <c r="A68">
-        <v>6</v>
+      <c r="A68" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="69">
@@ -9553,86 +9562,91 @@
     </row>
     <row r="70">
       <c r="A70">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71">
       <c r="A71">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72">
       <c r="A72">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
       <c r="A75">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76">
       <c r="A76">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78">
       <c r="A78">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82">
       <c r="A82">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83">
       <c r="A83">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84">
       <c r="A84">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85">
       <c r="A85">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
       <c r="A86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87">
         <v>1</v>
       </c>
     </row>

</xml_diff>